<commit_message>
correção do :id do listschoolClassAll, correção da rota Excel List Donates que não retornava nada
</commit_message>
<xml_diff>
--- a/donations.xlsx
+++ b/donations.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -80,75 +80,6 @@
   </si>
   <si>
     <t>createdAt</t>
-  </si>
-  <si>
-    <t>afc81039-1fd2-44b2-9048-329a819c21f4</t>
-  </si>
-  <si>
-    <t>Usuario 19062</t>
-  </si>
-  <si>
-    <t>usuario19062@hotmail.com</t>
-  </si>
-  <si>
-    <t>11982425569</t>
-  </si>
-  <si>
-    <t>neutral</t>
-  </si>
-  <si>
-    <t>11/08/1994</t>
-  </si>
-  <si>
-    <t>santiago</t>
-  </si>
-  <si>
-    <t>433</t>
-  </si>
-  <si>
-    <t>24A</t>
-  </si>
-  <si>
-    <t>gotham</t>
-  </si>
-  <si>
-    <t>03590-090</t>
-  </si>
-  <si>
-    <t>avenida del vino</t>
-  </si>
-  <si>
-    <t>00000019062</t>
-  </si>
-  <si>
-    <t>000019062</t>
-  </si>
-  <si>
-    <t>Sem informação ainda</t>
-  </si>
-  <si>
-    <t>canceled</t>
-  </si>
-  <si>
-    <t>cus_O6vERShiM3kz3G</t>
-  </si>
-  <si>
-    <t>e80efe90-3f67-48d9-80b0-3d777e64186b</t>
-  </si>
-  <si>
-    <t>Usuario 19063</t>
-  </si>
-  <si>
-    <t>usuario19063@hotmail.com</t>
-  </si>
-  <si>
-    <t>00000019063</t>
-  </si>
-  <si>
-    <t>000019063</t>
-  </si>
-  <si>
-    <t>cus_O6vm7gDAQKYhT8</t>
   </si>
 </sst>
 </file>
@@ -184,9 +115,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:W1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -598,142 +528,6 @@
       </c>
       <c r="W1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2">
-        <v>50</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="1">
-        <v>45096.52857282407</v>
-      </c>
-      <c r="U2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="1">
-        <v>45096.52857284722</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q3">
-        <v>50</v>
-      </c>
-      <c r="R3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" s="1">
-        <v>45096.55219487268</v>
-      </c>
-      <c r="U3" t="s">
-        <v>45</v>
-      </c>
-      <c r="W3" s="1">
-        <v>45096.55220209491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>